<commit_message>
changed some date/file handling, simplified Vintage for #86, closes #82
</commit_message>
<xml_diff>
--- a/output/kep.xlsx
+++ b/output/kep.xlsx
@@ -10719,12 +10719,54 @@
       <c r="H75">
         <v>101.3</v>
       </c>
+      <c r="I75">
+        <v>83.8</v>
+      </c>
+      <c r="K75">
+        <v>102.5</v>
+      </c>
+      <c r="L75">
+        <v>14443</v>
+      </c>
+      <c r="M75">
+        <v>7529.9</v>
+      </c>
+      <c r="N75">
+        <v>4611.6</v>
+      </c>
+      <c r="O75">
+        <v>14507.5</v>
+      </c>
+      <c r="P75">
+        <v>7122</v>
+      </c>
+      <c r="Q75">
+        <v>5049</v>
+      </c>
+      <c r="R75">
+        <v>-407.8</v>
+      </c>
+      <c r="S75">
+        <v>437.3</v>
+      </c>
+      <c r="T75">
+        <v>58.6</v>
+      </c>
       <c r="U75">
         <v>106.9</v>
       </c>
       <c r="V75">
         <v>103.8</v>
       </c>
+      <c r="W75">
+        <v>3521.5</v>
+      </c>
+      <c r="X75">
+        <v>159.3</v>
+      </c>
+      <c r="Y75">
+        <v>106.3</v>
+      </c>
       <c r="Z75">
         <v>3443.4</v>
       </c>
@@ -10759,13 +10801,13 @@
         <v>5.2</v>
       </c>
       <c r="AK75">
-        <v>40556</v>
+        <v>40712</v>
       </c>
       <c r="AL75">
-        <v>109.6</v>
+        <v>110</v>
       </c>
       <c r="AM75">
-        <v>103.1</v>
+        <v>103.4</v>
       </c>
     </row>
   </sheetData>
@@ -10775,7 +10817,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK223"/>
+  <dimension ref="A1:AK224"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -34587,6 +34629,36 @@
       <c r="H223">
         <v>100.6</v>
       </c>
+      <c r="I223">
+        <v>29.5</v>
+      </c>
+      <c r="J223">
+        <v>14443</v>
+      </c>
+      <c r="K223">
+        <v>7529.9</v>
+      </c>
+      <c r="L223">
+        <v>4611.6</v>
+      </c>
+      <c r="M223">
+        <v>14507.5</v>
+      </c>
+      <c r="N223">
+        <v>7122</v>
+      </c>
+      <c r="O223">
+        <v>5049</v>
+      </c>
+      <c r="P223">
+        <v>-407.8</v>
+      </c>
+      <c r="Q223">
+        <v>437.3</v>
+      </c>
+      <c r="R223">
+        <v>20.8</v>
+      </c>
       <c r="S223">
         <v>101.7</v>
       </c>
@@ -34621,19 +34693,93 @@
         <v>101.2</v>
       </c>
       <c r="AG223">
-        <v>430.8</v>
+        <v>431.2</v>
       </c>
       <c r="AH223">
         <v>5.1</v>
       </c>
       <c r="AI223">
-        <v>41640</v>
+        <v>42042</v>
       </c>
       <c r="AJ223">
-        <v>102.9</v>
+        <v>104.1</v>
       </c>
       <c r="AK223">
-        <v>102.9</v>
+        <v>103.9</v>
+      </c>
+    </row>
+    <row r="224" spans="1:37">
+      <c r="A224" s="2">
+        <v>42947</v>
+      </c>
+      <c r="B224">
+        <v>2017</v>
+      </c>
+      <c r="C224">
+        <v>7</v>
+      </c>
+      <c r="D224">
+        <v>100.1</v>
+      </c>
+      <c r="E224">
+        <v>98.90000000000001</v>
+      </c>
+      <c r="F224">
+        <v>100.1</v>
+      </c>
+      <c r="G224">
+        <v>101.6</v>
+      </c>
+      <c r="H224">
+        <v>100.1</v>
+      </c>
+      <c r="S224">
+        <v>97.5</v>
+      </c>
+      <c r="T224">
+        <v>101.1</v>
+      </c>
+      <c r="X224">
+        <v>1206.2</v>
+      </c>
+      <c r="Y224">
+        <v>104.6</v>
+      </c>
+      <c r="Z224">
+        <v>100.1</v>
+      </c>
+      <c r="AA224">
+        <v>1298.8</v>
+      </c>
+      <c r="AB224">
+        <v>103.1</v>
+      </c>
+      <c r="AC224">
+        <v>101.9</v>
+      </c>
+      <c r="AD224">
+        <v>2505</v>
+      </c>
+      <c r="AE224">
+        <v>103.8</v>
+      </c>
+      <c r="AF224">
+        <v>101</v>
+      </c>
+      <c r="AG224">
+        <v>441.9</v>
+      </c>
+      <c r="AH224">
+        <v>5.1</v>
+      </c>
+      <c r="AI224">
+        <v>39355</v>
+      </c>
+      <c r="AJ224">
+        <v>93.40000000000001</v>
+      </c>
+      <c r="AK224">
+        <v>104.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>